<commit_message>
bug de tema materia vacio
</commit_message>
<xml_diff>
--- a/ArchivosParaPruebas/DocentesImportacionMasiva.xlsx
+++ b/ArchivosParaPruebas/DocentesImportacionMasiva.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DayClass\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DayClass\ArchivosParaPruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59D4D1CF-84D0-4FAF-A243-3FF5BCD3951E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4324B6E-CA57-4E8C-83DF-8E7842CED2D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CC8C8EFF-2A13-4B52-AAD4-E9CF4F476D65}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="183">
   <si>
     <t>DNI</t>
   </si>
@@ -391,16 +391,205 @@
   </si>
   <si>
     <t>Lillith</t>
+  </si>
+  <si>
+    <t>PR90000</t>
+  </si>
+  <si>
+    <t>PR90001</t>
+  </si>
+  <si>
+    <t>PR90002</t>
+  </si>
+  <si>
+    <t>PR90003</t>
+  </si>
+  <si>
+    <t>PR90004</t>
+  </si>
+  <si>
+    <t>PR90005</t>
+  </si>
+  <si>
+    <t>PR90006</t>
+  </si>
+  <si>
+    <t>PR90007</t>
+  </si>
+  <si>
+    <t>PR90008</t>
+  </si>
+  <si>
+    <t>PR90009</t>
+  </si>
+  <si>
+    <t>PR90010</t>
+  </si>
+  <si>
+    <t>PR90011</t>
+  </si>
+  <si>
+    <t>PR90012</t>
+  </si>
+  <si>
+    <t>PR90013</t>
+  </si>
+  <si>
+    <t>PR90014</t>
+  </si>
+  <si>
+    <t>PR90015</t>
+  </si>
+  <si>
+    <t>PR90016</t>
+  </si>
+  <si>
+    <t>PR90017</t>
+  </si>
+  <si>
+    <t>PR90018</t>
+  </si>
+  <si>
+    <t>PR90019</t>
+  </si>
+  <si>
+    <t>PR90020</t>
+  </si>
+  <si>
+    <t>PR90021</t>
+  </si>
+  <si>
+    <t>PR90022</t>
+  </si>
+  <si>
+    <t>PR90023</t>
+  </si>
+  <si>
+    <t>PR90024</t>
+  </si>
+  <si>
+    <t>PR90025</t>
+  </si>
+  <si>
+    <t>PR90026</t>
+  </si>
+  <si>
+    <t>PR90027</t>
+  </si>
+  <si>
+    <t>PR90028</t>
+  </si>
+  <si>
+    <t>PR90029</t>
+  </si>
+  <si>
+    <t>PR90030</t>
+  </si>
+  <si>
+    <t>PR90031</t>
+  </si>
+  <si>
+    <t>PR90032</t>
+  </si>
+  <si>
+    <t>PR90033</t>
+  </si>
+  <si>
+    <t>PR90034</t>
+  </si>
+  <si>
+    <t>PR90035</t>
+  </si>
+  <si>
+    <t>PR90036</t>
+  </si>
+  <si>
+    <t>PR90037</t>
+  </si>
+  <si>
+    <t>PR90038</t>
+  </si>
+  <si>
+    <t>PR90039</t>
+  </si>
+  <si>
+    <t>PR90040</t>
+  </si>
+  <si>
+    <t>PR90041</t>
+  </si>
+  <si>
+    <t>PR90042</t>
+  </si>
+  <si>
+    <t>PR90043</t>
+  </si>
+  <si>
+    <t>PR90044</t>
+  </si>
+  <si>
+    <t>PR90045</t>
+  </si>
+  <si>
+    <t>PR90046</t>
+  </si>
+  <si>
+    <t>PR90047</t>
+  </si>
+  <si>
+    <t>PR90048</t>
+  </si>
+  <si>
+    <t>PR90049</t>
+  </si>
+  <si>
+    <t>PR90050</t>
+  </si>
+  <si>
+    <t>PR90051</t>
+  </si>
+  <si>
+    <t>PR90052</t>
+  </si>
+  <si>
+    <t>PR90053</t>
+  </si>
+  <si>
+    <t>PR90054</t>
+  </si>
+  <si>
+    <t>PR90055</t>
+  </si>
+  <si>
+    <t>PR90056</t>
+  </si>
+  <si>
+    <t>PR90057</t>
+  </si>
+  <si>
+    <t>PR90058</t>
+  </si>
+  <si>
+    <t>PR90059</t>
+  </si>
+  <si>
+    <t>PR90060</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -760,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBF6917-7B94-4C15-A867-E4346E5FD415}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D62"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,8 +973,8 @@
       <c r="A2" s="1">
         <v>14248800</v>
       </c>
-      <c r="B2" s="1">
-        <v>90000</v>
+      <c r="B2" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -798,8 +987,8 @@
       <c r="A3" s="1">
         <v>23234845</v>
       </c>
-      <c r="B3" s="1">
-        <v>90001</v>
+      <c r="B3" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -812,8 +1001,8 @@
       <c r="A4" s="1">
         <v>11700237</v>
       </c>
-      <c r="B4" s="1">
-        <v>90002</v>
+      <c r="B4" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
@@ -826,8 +1015,8 @@
       <c r="A5" s="1">
         <v>16529441</v>
       </c>
-      <c r="B5" s="1">
-        <v>90003</v>
+      <c r="B5" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
@@ -840,8 +1029,8 @@
       <c r="A6" s="1">
         <v>21669268</v>
       </c>
-      <c r="B6" s="1">
-        <v>90004</v>
+      <c r="B6" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -854,8 +1043,8 @@
       <c r="A7" s="1">
         <v>20684890</v>
       </c>
-      <c r="B7" s="1">
-        <v>90005</v>
+      <c r="B7" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -868,8 +1057,8 @@
       <c r="A8" s="1">
         <v>14467596</v>
       </c>
-      <c r="B8" s="1">
-        <v>90006</v>
+      <c r="B8" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>16</v>
@@ -882,8 +1071,8 @@
       <c r="A9" s="1">
         <v>11537358</v>
       </c>
-      <c r="B9" s="1">
-        <v>90007</v>
+      <c r="B9" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>18</v>
@@ -896,8 +1085,8 @@
       <c r="A10" s="1">
         <v>20609060</v>
       </c>
-      <c r="B10" s="1">
-        <v>90008</v>
+      <c r="B10" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>20</v>
@@ -910,8 +1099,8 @@
       <c r="A11" s="1">
         <v>19617326</v>
       </c>
-      <c r="B11" s="1">
-        <v>90009</v>
+      <c r="B11" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>22</v>
@@ -924,8 +1113,8 @@
       <c r="A12" s="1">
         <v>12618030</v>
       </c>
-      <c r="B12" s="1">
-        <v>90010</v>
+      <c r="B12" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>24</v>
@@ -938,8 +1127,8 @@
       <c r="A13" s="1">
         <v>24157590</v>
       </c>
-      <c r="B13" s="1">
-        <v>90011</v>
+      <c r="B13" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>26</v>
@@ -952,8 +1141,8 @@
       <c r="A14" s="1">
         <v>15151583</v>
       </c>
-      <c r="B14" s="1">
-        <v>90012</v>
+      <c r="B14" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
@@ -966,8 +1155,8 @@
       <c r="A15" s="1">
         <v>24306617</v>
       </c>
-      <c r="B15" s="1">
-        <v>90013</v>
+      <c r="B15" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>30</v>
@@ -980,8 +1169,8 @@
       <c r="A16" s="1">
         <v>23758230</v>
       </c>
-      <c r="B16" s="1">
-        <v>90014</v>
+      <c r="B16" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -994,8 +1183,8 @@
       <c r="A17" s="1">
         <v>15630879</v>
       </c>
-      <c r="B17" s="1">
-        <v>90015</v>
+      <c r="B17" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>34</v>
@@ -1008,8 +1197,8 @@
       <c r="A18" s="1">
         <v>15583560</v>
       </c>
-      <c r="B18" s="1">
-        <v>90016</v>
+      <c r="B18" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>36</v>
@@ -1022,8 +1211,8 @@
       <c r="A19" s="1">
         <v>14187665</v>
       </c>
-      <c r="B19" s="1">
-        <v>90017</v>
+      <c r="B19" s="1" t="s">
+        <v>139</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>38</v>
@@ -1036,8 +1225,8 @@
       <c r="A20" s="1">
         <v>19763883</v>
       </c>
-      <c r="B20" s="1">
-        <v>90018</v>
+      <c r="B20" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>40</v>
@@ -1050,8 +1239,8 @@
       <c r="A21" s="1">
         <v>17032877</v>
       </c>
-      <c r="B21" s="1">
-        <v>90019</v>
+      <c r="B21" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>42</v>
@@ -1064,8 +1253,8 @@
       <c r="A22" s="1">
         <v>24904907</v>
       </c>
-      <c r="B22" s="1">
-        <v>90020</v>
+      <c r="B22" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>44</v>
@@ -1078,8 +1267,8 @@
       <c r="A23" s="1">
         <v>19247224</v>
       </c>
-      <c r="B23" s="1">
-        <v>90021</v>
+      <c r="B23" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>46</v>
@@ -1092,8 +1281,8 @@
       <c r="A24" s="1">
         <v>13206018</v>
       </c>
-      <c r="B24" s="1">
-        <v>90022</v>
+      <c r="B24" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>48</v>
@@ -1106,8 +1295,8 @@
       <c r="A25" s="1">
         <v>11080178</v>
       </c>
-      <c r="B25" s="1">
-        <v>90023</v>
+      <c r="B25" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>50</v>
@@ -1120,8 +1309,8 @@
       <c r="A26" s="1">
         <v>10725176</v>
       </c>
-      <c r="B26" s="1">
-        <v>90024</v>
+      <c r="B26" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>52</v>
@@ -1134,8 +1323,8 @@
       <c r="A27" s="1">
         <v>16572676</v>
       </c>
-      <c r="B27" s="1">
-        <v>90025</v>
+      <c r="B27" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>54</v>
@@ -1148,8 +1337,8 @@
       <c r="A28" s="1">
         <v>12921202</v>
       </c>
-      <c r="B28" s="1">
-        <v>90026</v>
+      <c r="B28" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>56</v>
@@ -1162,8 +1351,8 @@
       <c r="A29" s="1">
         <v>20277607</v>
       </c>
-      <c r="B29" s="1">
-        <v>90027</v>
+      <c r="B29" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>58</v>
@@ -1176,8 +1365,8 @@
       <c r="A30" s="1">
         <v>24842771</v>
       </c>
-      <c r="B30" s="1">
-        <v>90028</v>
+      <c r="B30" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>60</v>
@@ -1190,8 +1379,8 @@
       <c r="A31" s="1">
         <v>24602983</v>
       </c>
-      <c r="B31" s="1">
-        <v>90029</v>
+      <c r="B31" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>61</v>
@@ -1204,8 +1393,8 @@
       <c r="A32" s="1">
         <v>13667844</v>
       </c>
-      <c r="B32" s="1">
-        <v>90030</v>
+      <c r="B32" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>63</v>
@@ -1218,8 +1407,8 @@
       <c r="A33" s="1">
         <v>14628685</v>
       </c>
-      <c r="B33" s="1">
-        <v>90031</v>
+      <c r="B33" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>33</v>
@@ -1232,8 +1421,8 @@
       <c r="A34" s="1">
         <v>20318629</v>
       </c>
-      <c r="B34" s="1">
-        <v>90032</v>
+      <c r="B34" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>66</v>
@@ -1246,8 +1435,8 @@
       <c r="A35" s="1">
         <v>20752043</v>
       </c>
-      <c r="B35" s="1">
-        <v>90033</v>
+      <c r="B35" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>68</v>
@@ -1260,8 +1449,8 @@
       <c r="A36" s="1">
         <v>20574466</v>
       </c>
-      <c r="B36" s="1">
-        <v>90034</v>
+      <c r="B36" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>70</v>
@@ -1274,8 +1463,8 @@
       <c r="A37" s="1">
         <v>19085599</v>
       </c>
-      <c r="B37" s="1">
-        <v>90035</v>
+      <c r="B37" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>72</v>
@@ -1288,8 +1477,8 @@
       <c r="A38" s="1">
         <v>23803239</v>
       </c>
-      <c r="B38" s="1">
-        <v>90036</v>
+      <c r="B38" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>74</v>
@@ -1302,8 +1491,8 @@
       <c r="A39" s="1">
         <v>19947972</v>
       </c>
-      <c r="B39" s="1">
-        <v>90037</v>
+      <c r="B39" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>76</v>
@@ -1316,8 +1505,8 @@
       <c r="A40" s="1">
         <v>23523841</v>
       </c>
-      <c r="B40" s="1">
-        <v>90038</v>
+      <c r="B40" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>78</v>
@@ -1330,8 +1519,8 @@
       <c r="A41" s="1">
         <v>23432540</v>
       </c>
-      <c r="B41" s="1">
-        <v>90039</v>
+      <c r="B41" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>80</v>
@@ -1344,8 +1533,8 @@
       <c r="A42" s="1">
         <v>21262344</v>
       </c>
-      <c r="B42" s="1">
-        <v>90040</v>
+      <c r="B42" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>82</v>
@@ -1358,8 +1547,8 @@
       <c r="A43" s="1">
         <v>21185275</v>
       </c>
-      <c r="B43" s="1">
-        <v>90041</v>
+      <c r="B43" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>84</v>
@@ -1372,8 +1561,8 @@
       <c r="A44" s="1">
         <v>10462925</v>
       </c>
-      <c r="B44" s="1">
-        <v>90042</v>
+      <c r="B44" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>86</v>
@@ -1386,8 +1575,8 @@
       <c r="A45" s="1">
         <v>17350654</v>
       </c>
-      <c r="B45" s="1">
-        <v>90043</v>
+      <c r="B45" s="1" t="s">
+        <v>165</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>88</v>
@@ -1400,8 +1589,8 @@
       <c r="A46" s="1">
         <v>20557761</v>
       </c>
-      <c r="B46" s="1">
-        <v>90044</v>
+      <c r="B46" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>90</v>
@@ -1414,8 +1603,8 @@
       <c r="A47" s="1">
         <v>11546781</v>
       </c>
-      <c r="B47" s="1">
-        <v>90045</v>
+      <c r="B47" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>90</v>
@@ -1428,8 +1617,8 @@
       <c r="A48" s="1">
         <v>18531701</v>
       </c>
-      <c r="B48" s="1">
-        <v>90046</v>
+      <c r="B48" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>93</v>
@@ -1442,8 +1631,8 @@
       <c r="A49" s="1">
         <v>15395201</v>
       </c>
-      <c r="B49" s="1">
-        <v>90047</v>
+      <c r="B49" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>95</v>
@@ -1456,8 +1645,8 @@
       <c r="A50" s="1">
         <v>16763857</v>
       </c>
-      <c r="B50" s="1">
-        <v>90048</v>
+      <c r="B50" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>96</v>
@@ -1470,8 +1659,8 @@
       <c r="A51" s="1">
         <v>10892106</v>
       </c>
-      <c r="B51" s="1">
-        <v>90049</v>
+      <c r="B51" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>98</v>
@@ -1484,8 +1673,8 @@
       <c r="A52" s="1">
         <v>22865049</v>
       </c>
-      <c r="B52" s="1">
-        <v>90050</v>
+      <c r="B52" s="1" t="s">
+        <v>172</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>100</v>
@@ -1498,8 +1687,8 @@
       <c r="A53" s="1">
         <v>20484134</v>
       </c>
-      <c r="B53" s="1">
-        <v>90051</v>
+      <c r="B53" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>102</v>
@@ -1512,8 +1701,8 @@
       <c r="A54" s="1">
         <v>15838695</v>
       </c>
-      <c r="B54" s="1">
-        <v>90052</v>
+      <c r="B54" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>104</v>
@@ -1526,8 +1715,8 @@
       <c r="A55" s="1">
         <v>12406334</v>
       </c>
-      <c r="B55" s="1">
-        <v>90053</v>
+      <c r="B55" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>106</v>
@@ -1540,8 +1729,8 @@
       <c r="A56" s="1">
         <v>16737751</v>
       </c>
-      <c r="B56" s="1">
-        <v>90054</v>
+      <c r="B56" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>108</v>
@@ -1554,8 +1743,8 @@
       <c r="A57" s="1">
         <v>12809807</v>
       </c>
-      <c r="B57" s="1">
-        <v>90055</v>
+      <c r="B57" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>110</v>
@@ -1568,8 +1757,8 @@
       <c r="A58" s="1">
         <v>11865383</v>
       </c>
-      <c r="B58" s="1">
-        <v>90056</v>
+      <c r="B58" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>112</v>
@@ -1582,8 +1771,8 @@
       <c r="A59" s="1">
         <v>18306692</v>
       </c>
-      <c r="B59" s="1">
-        <v>90057</v>
+      <c r="B59" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>114</v>
@@ -1596,8 +1785,8 @@
       <c r="A60" s="1">
         <v>12295784</v>
       </c>
-      <c r="B60" s="1">
-        <v>90058</v>
+      <c r="B60" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>116</v>
@@ -1610,8 +1799,8 @@
       <c r="A61" s="1">
         <v>11858591</v>
       </c>
-      <c r="B61" s="1">
-        <v>90059</v>
+      <c r="B61" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>118</v>
@@ -1624,8 +1813,8 @@
       <c r="A62" s="1">
         <v>19115260</v>
       </c>
-      <c r="B62" s="1">
-        <v>90060</v>
+      <c r="B62" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>120</v>
@@ -1635,6 +1824,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>